<commit_message>
- Organized Asset files better. - RewardCard UserControl now functional - Excel lists completed. - Added Rings. - Created more screens for Rags to Riches
</commit_message>
<xml_diff>
--- a/PVPlayTool/Data/DaS_Items.xlsx
+++ b/PVPlayTool/Data/DaS_Items.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="38">
   <si>
     <t>Item Name</t>
   </si>
@@ -84,6 +84,60 @@
   </si>
   <si>
     <t>Silver Pendant</t>
+  </si>
+  <si>
+    <t>ImagePath</t>
+  </si>
+  <si>
+    <t>tex_DaS_Humanity.png</t>
+  </si>
+  <si>
+    <t>tex_DaS_GreenBlossom.png</t>
+  </si>
+  <si>
+    <t>tex_DaS_BloodredMossClump.png</t>
+  </si>
+  <si>
+    <t>tex_DaS_PurpleMossClump.png</t>
+  </si>
+  <si>
+    <t>tex_DaS_BloomingPurpleMossClump.png</t>
+  </si>
+  <si>
+    <t>tex_DaS_CharcoalPineResin.png</t>
+  </si>
+  <si>
+    <t>tex_DaS_RottenPineResin.png</t>
+  </si>
+  <si>
+    <t>tex_DaS_GoldPineResin.png</t>
+  </si>
+  <si>
+    <t>tex_DaS_Elizabeth'sMushroom.png</t>
+  </si>
+  <si>
+    <t>tex_DaS_DivineBlessing.png</t>
+  </si>
+  <si>
+    <t>tex_DaS_Firebomb.png</t>
+  </si>
+  <si>
+    <t>tex_DaS_BlackFirebomb.png</t>
+  </si>
+  <si>
+    <t>tex_DaS_DungPie.png</t>
+  </si>
+  <si>
+    <t>tex_DaS_ThrowingKnife.png</t>
+  </si>
+  <si>
+    <t>tex_DaS_PoisonThrowingKnife.png</t>
+  </si>
+  <si>
+    <t>tex_DaS_Lloyd'sTalisman.png</t>
+  </si>
+  <si>
+    <t>tex_DaS_SilverPendant.png</t>
   </si>
 </sst>
 </file>
@@ -410,18 +464,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+      <selection activeCell="E2" sqref="E2:E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="65.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -431,8 +487,11 @@
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -442,8 +501,11 @@
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -453,8 +515,11 @@
       <c r="C3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -464,8 +529,11 @@
       <c r="C4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -475,8 +543,11 @@
       <c r="C5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -486,8 +557,11 @@
       <c r="C6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -497,8 +571,11 @@
       <c r="C7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -508,8 +585,11 @@
       <c r="C8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -519,8 +599,11 @@
       <c r="C9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -530,8 +613,11 @@
       <c r="C10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -541,8 +627,11 @@
       <c r="C11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -552,8 +641,11 @@
       <c r="C12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -563,8 +655,11 @@
       <c r="C13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -574,8 +669,11 @@
       <c r="C14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -585,8 +683,11 @@
       <c r="C15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -596,8 +697,11 @@
       <c r="C16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -607,8 +711,11 @@
       <c r="C17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -618,8 +725,11 @@
       <c r="C18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -629,8 +739,11 @@
       <c r="C19">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -640,8 +753,11 @@
       <c r="C20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -651,8 +767,11 @@
       <c r="C21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -662,8 +781,11 @@
       <c r="C22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -673,8 +795,11 @@
       <c r="C23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -684,8 +809,11 @@
       <c r="C24">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -695,8 +823,11 @@
       <c r="C25">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -706,8 +837,11 @@
       <c r="C26">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -717,8 +851,11 @@
       <c r="C27">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -728,8 +865,11 @@
       <c r="C28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>13</v>
       </c>
@@ -739,8 +879,11 @@
       <c r="C29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -750,8 +893,11 @@
       <c r="C30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -761,8 +907,11 @@
       <c r="C31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -772,8 +921,11 @@
       <c r="C32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -783,8 +935,11 @@
       <c r="C33">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>15</v>
       </c>
@@ -794,8 +949,11 @@
       <c r="C34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>15</v>
       </c>
@@ -805,8 +963,11 @@
       <c r="C35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>15</v>
       </c>
@@ -816,8 +977,11 @@
       <c r="C36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -827,8 +991,11 @@
       <c r="C37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -838,8 +1005,11 @@
       <c r="C38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>16</v>
       </c>
@@ -849,8 +1019,11 @@
       <c r="C39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>17</v>
       </c>
@@ -860,8 +1033,11 @@
       <c r="C40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>17</v>
       </c>
@@ -871,8 +1047,11 @@
       <c r="C41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>17</v>
       </c>
@@ -882,8 +1061,11 @@
       <c r="C42">
         <v>2</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>18</v>
       </c>
@@ -893,8 +1075,11 @@
       <c r="C43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>18</v>
       </c>
@@ -904,8 +1089,11 @@
       <c r="C44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>18</v>
       </c>
@@ -915,8 +1103,11 @@
       <c r="C45">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>19</v>
       </c>
@@ -925,6 +1116,9 @@
       </c>
       <c r="C46">
         <v>2</v>
+      </c>
+      <c r="D46" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>